<commit_message>
added assign user starting points
</commit_message>
<xml_diff>
--- a/Ecom Modelling Costa.xlsx
+++ b/Ecom Modelling Costa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmclaughlin/Library/CloudStorage/OneDrive-SubtvU/Alex-McLaughlin/Loyality Scheme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863574AC-46A0-4F41-A3D0-56C2B90B5A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ECF4D6-0FA4-9B4F-BFB3-1729381C8718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{A0095DDC-8E5F-8542-BAAD-5C4BF5024CD1}"/>
+    <workbookView xWindow="2880" yWindow="880" windowWidth="30240" windowHeight="17720" xr2:uid="{A0095DDC-8E5F-8542-BAAD-5C4BF5024CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -806,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E321E73A-F259-E94B-B600-4AEF6EA281B8}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>

</xml_diff>